<commit_message>
add table to excel file
</commit_message>
<xml_diff>
--- a/Document/MyDocument/11月.xlsx
+++ b/Document/MyDocument/11月.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="19420" windowHeight="9450"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="10" sheetId="1" r:id="rId1"/>
     <sheet name="11" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>10月份记录</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -39,6 +38,10 @@
   </si>
   <si>
     <t>唐浩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11月份记录</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -402,16 +405,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G24" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -872,349 +875,230 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>43374</v>
+        <v>43405</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>43375</v>
+        <v>43406</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>43376</v>
+        <v>43407</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>43377</v>
+        <v>43408</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>43378</v>
+        <v>43409</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>43379</v>
+        <v>43410</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>43380</v>
+        <v>43411</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>43381</v>
+        <v>43412</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>43382</v>
+        <v>43413</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>43383</v>
+        <v>43414</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>43384</v>
+        <v>43415</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>43385</v>
+        <v>43416</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>43386</v>
+        <v>43417</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>43387</v>
+        <v>43418</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>43388</v>
+        <v>43419</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>43389</v>
+        <v>43420</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>43390</v>
+        <v>43421</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>43391</v>
+        <v>43422</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>43392</v>
+        <v>43423</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
-        <v>43393</v>
+        <v>43424</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
-        <v>43394</v>
+        <v>43425</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
-        <v>43395</v>
+        <v>43426</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>43427</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2">
+      <c r="B25" s="2">
         <v>3.5</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="1">
-        <v>43397</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5">
+        <v>43428</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="1">
-        <v>43398</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5">
+        <v>43429</v>
+      </c>
+      <c r="B27" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1">
-        <v>43399</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5">
+        <v>43430</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="1">
-        <v>43400</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5">
+        <v>43431</v>
+      </c>
+      <c r="B29" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1">
-        <v>43401</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5">
+        <v>43432</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1">
-        <v>43402</v>
+        <v>43433</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5">
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="1">
-        <v>43403</v>
+        <v>43434</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1">
-        <v>43404</v>
-      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>